<commit_message>
fixed typo 'duration og vomiting' -> 'duration of vomiting'
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@69878 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/PRISM_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/PRISM_metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="24240" windowHeight="11775" tabRatio="922" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="24240" windowHeight="11775" tabRatio="922" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PRISM classes" sheetId="19" r:id="rId1"/>
@@ -8283,9 +8283,6 @@
     <t>all terms added with annotationProp, "term type" ICEMR_0000025, with value 'value'</t>
   </si>
   <si>
-    <t>duration og vomiting</t>
-  </si>
-  <si>
     <t>ICEMR_0000028</t>
   </si>
   <si>
@@ -8308,6 +8305,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/EUPATH_0000134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        duration of vomiting</t>
   </si>
 </sst>
 </file>
@@ -13176,7 +13176,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13186,8 +13186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G287"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A90" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -13216,32 +13216,32 @@
         <v>1782</v>
       </c>
       <c r="E1" s="154" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="F1" s="154" t="s">
         <v>1784</v>
       </c>
       <c r="G1" s="154" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="155" customFormat="1" ht="15.75">
       <c r="A2" s="154"/>
       <c r="B2" s="154"/>
       <c r="C2" s="154" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D2" s="154" t="s">
         <v>1835</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="E2" s="154" t="s">
+        <v>1839</v>
+      </c>
+      <c r="F2" s="154" t="s">
         <v>1836</v>
       </c>
-      <c r="E2" s="154" t="s">
+      <c r="G2" s="154" t="s">
         <v>1840</v>
-      </c>
-      <c r="F2" s="154" t="s">
-        <v>1837</v>
-      </c>
-      <c r="G2" s="154" t="s">
-        <v>1841</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -14189,7 +14189,7 @@
     </row>
     <row r="44" spans="1:7" s="13" customFormat="1">
       <c r="A44" s="143" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="B44" s="87" t="s">
         <v>1733</v>
@@ -15794,7 +15794,7 @@
         <v>181</v>
       </c>
       <c r="E119" s="152" t="s">
-        <v>1834</v>
+        <v>1206</v>
       </c>
       <c r="F119" s="87"/>
       <c r="G119" s="87"/>
@@ -17137,7 +17137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
@@ -17162,15 +17162,15 @@
         <v>1782</v>
       </c>
       <c r="D1" s="154" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="148" customFormat="1" ht="15.75">
       <c r="C2" s="154" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="D2" s="154" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="E2" s="154"/>
       <c r="F2" s="154"/>
@@ -28342,11 +28342,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T287"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="I243" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="I222" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J259" sqref="J259"/>
+      <selection pane="bottomRight" activeCell="I229" sqref="I229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -31760,10 +31760,10 @@
         <v>1235</v>
       </c>
       <c r="L106" s="143" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="M106" s="143" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="N106" s="10" t="s">
         <v>316</v>
@@ -36369,7 +36369,7 @@
         <v>181</v>
       </c>
       <c r="I222" s="63" t="s">
-        <v>820</v>
+        <v>1842</v>
       </c>
       <c r="J222" s="3" t="s">
         <v>197</v>
@@ -37914,10 +37914,10 @@
   <dimension ref="A1:K294"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="D247" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="D222" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H264" sqref="H264"/>
+      <selection pane="bottomRight" activeCell="E222" sqref="E222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -40189,7 +40189,7 @@
         <v>1235</v>
       </c>
       <c r="H106" s="143" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="I106" s="10" t="s">
         <v>316</v>
@@ -42947,7 +42947,7 @@
         <v>181</v>
       </c>
       <c r="E222" s="63" t="s">
-        <v>820</v>
+        <v>1842</v>
       </c>
       <c r="F222" s="3" t="s">
         <v>197</v>

</xml_diff>

<commit_message>
Fixed typo: Uunfed -> unfed
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@70051 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/PRISM_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/PRISM_metadata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11873" uniqueCount="1857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11873" uniqueCount="1859">
   <si>
     <t>abdominal pain</t>
   </si>
@@ -8351,6 +8351,36 @@
   </si>
   <si>
     <t>PRISM data dictionary label (en)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unfed </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A. gambiae</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Unfed</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A. funestus</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -13226,7 +13256,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13236,8 +13266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G287"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -14363,7 +14393,7 @@
         <v>306</v>
       </c>
       <c r="D49" s="87" t="s">
-        <v>1788</v>
+        <v>1857</v>
       </c>
       <c r="E49" s="86" t="s">
         <v>722</v>
@@ -14478,7 +14508,7 @@
         <v>305</v>
       </c>
       <c r="D54" s="87" t="s">
-        <v>1792</v>
+        <v>1858</v>
       </c>
       <c r="E54" s="86" t="s">
         <v>727</v>

</xml_diff>

<commit_message>
Add hospital name mapping between the cleaned up list provided by San James and the terms actually used in the database
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@70563 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/PRISM_metadata.xlsx
+++ b/Load/src/ontology/ICEMR/PRISM_metadata.xlsx
@@ -4,31 +4,32 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="24240" windowHeight="11595" tabRatio="922" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="24240" windowHeight="11595" tabRatio="922"/>
   </bookViews>
   <sheets>
     <sheet name="PRISM classes" sheetId="19" r:id="rId1"/>
     <sheet name="PRISM individuals" sheetId="20" r:id="rId2"/>
-    <sheet name="dataDictionary2display" sheetId="22" r:id="rId3"/>
-    <sheet name="Proposed Revision" sheetId="4" r:id="rId4"/>
-    <sheet name="Proposed Revision_ontology" sheetId="5" r:id="rId5"/>
-    <sheet name="Proposed Revision_ontology IRIs" sheetId="18" r:id="rId6"/>
-    <sheet name="PRISMCuratedRelationships" sheetId="8" r:id="rId7"/>
-    <sheet name="PRISMCuratedSynonyms" sheetId="11" r:id="rId8"/>
-    <sheet name="PRISMCuratedTerms" sheetId="12" r:id="rId9"/>
-    <sheet name="duplicate" sheetId="21" r:id="rId10"/>
+    <sheet name="hospital mapping" sheetId="23" r:id="rId3"/>
+    <sheet name="dataDictionary2display" sheetId="22" r:id="rId4"/>
+    <sheet name="Proposed Revision" sheetId="4" r:id="rId5"/>
+    <sheet name="Proposed Revision_ontology" sheetId="5" r:id="rId6"/>
+    <sheet name="Proposed Revision_ontology IRIs" sheetId="18" r:id="rId7"/>
+    <sheet name="PRISMCuratedRelationships" sheetId="8" r:id="rId8"/>
+    <sheet name="PRISMCuratedSynonyms" sheetId="11" r:id="rId9"/>
+    <sheet name="PRISMCuratedTerms" sheetId="12" r:id="rId10"/>
+    <sheet name="duplicate" sheetId="21" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Proposed Revision'!$A$3:$Y$194</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Proposed Revision_ontology'!$A$3:$T$271</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Proposed Revision_ontology IRIs'!$A$3:$K$278</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Proposed Revision'!$A$3:$Y$194</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Proposed Revision_ontology'!$A$3:$T$271</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Proposed Revision_ontology IRIs'!$A$3:$K$278</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13645" uniqueCount="2626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13681" uniqueCount="2644">
   <si>
     <t>abdominal pain</t>
   </si>
@@ -10683,6 +10684,60 @@
   </si>
   <si>
     <t>When IRI is not provided, the temporal term will be generated with assigned ID like TEMP_XXXXX. These terms also has corresponding ontology terms as Related Synonym listed in Column E</t>
+  </si>
+  <si>
+    <t>bwindi hospital</t>
+  </si>
+  <si>
+    <t>jinja hospital</t>
+  </si>
+  <si>
+    <t>kauka healthy centre</t>
+  </si>
+  <si>
+    <t>kihihi h c iv</t>
+  </si>
+  <si>
+    <t>kihihi h/c</t>
+  </si>
+  <si>
+    <t>kihihi h/c iv</t>
+  </si>
+  <si>
+    <t>kihihi hc</t>
+  </si>
+  <si>
+    <t>kihihi hc iv</t>
+  </si>
+  <si>
+    <t>kihihi health centre 1v</t>
+  </si>
+  <si>
+    <t>kihihi health centre iv</t>
+  </si>
+  <si>
+    <t>nagonera h/c iv</t>
+  </si>
+  <si>
+    <t>nagongera h/c iv</t>
+  </si>
+  <si>
+    <t>nagongera h/civ</t>
+  </si>
+  <si>
+    <t>nagongera hc iv</t>
+  </si>
+  <si>
+    <t>nagongera hciv</t>
+  </si>
+  <si>
+    <t>nagongera health centre iv</t>
+  </si>
+  <si>
+    <t>tdh</t>
+  </si>
+  <si>
+    <t>tororo hospital</t>
   </si>
 </sst>
 </file>
@@ -15602,7 +15657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -15612,7 +15667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G298"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
     </sheetView>
@@ -19722,6 +19777,579 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1554</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" t="s">
+        <v>602</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1555</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B5" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B6" t="s">
+        <v>456</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1557</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>457</v>
+      </c>
+      <c r="B7" t="s">
+        <v>457</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1558</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B8" t="s">
+        <v>455</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1559</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" t="s">
+        <v>676</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>329</v>
+      </c>
+      <c r="B10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" t="s">
+        <v>330</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>335</v>
+      </c>
+      <c r="B12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" t="s">
+        <v>332</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>333</v>
+      </c>
+      <c r="B14" t="s">
+        <v>333</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B15" t="s">
+        <v>334</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" t="s">
+        <v>336</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" t="s">
+        <v>337</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>465</v>
+      </c>
+      <c r="B18" t="s">
+        <v>465</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>428</v>
+      </c>
+      <c r="B19" t="s">
+        <v>428</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>521</v>
+      </c>
+      <c r="B20" t="s">
+        <v>521</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" t="s">
+        <v>226</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>840</v>
+      </c>
+      <c r="B23" t="s">
+        <v>840</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>518</v>
+      </c>
+      <c r="B24" t="s">
+        <v>518</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>788</v>
+      </c>
+      <c r="B25" t="s">
+        <v>788</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>430</v>
+      </c>
+      <c r="B26" t="s">
+        <v>430</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B27" t="s">
+        <v>322</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>519</v>
+      </c>
+      <c r="B28" t="s">
+        <v>519</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>839</v>
+      </c>
+      <c r="B30" t="s">
+        <v>839</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>520</v>
+      </c>
+      <c r="B31" t="s">
+        <v>520</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>1454</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1454</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1480</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>1456</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1456</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>431</v>
+      </c>
+      <c r="B35" t="s">
+        <v>431</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>786</v>
+      </c>
+      <c r="B36" t="s">
+        <v>786</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>314</v>
+      </c>
+      <c r="B37" t="s">
+        <v>314</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>315</v>
+      </c>
+      <c r="B38" t="s">
+        <v>315</v>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>313</v>
+      </c>
+      <c r="B39" t="s">
+        <v>313</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>787</v>
+      </c>
+      <c r="B40" t="s">
+        <v>787</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>523</v>
+      </c>
+      <c r="B41" t="s">
+        <v>523</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>836</v>
+      </c>
+      <c r="B42" t="s">
+        <v>836</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>524</v>
+      </c>
+      <c r="B43" t="s">
+        <v>524</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>522</v>
+      </c>
+      <c r="B44" t="s">
+        <v>522</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>807</v>
+      </c>
+      <c r="B45" t="s">
+        <v>807</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B46" t="s">
+        <v>343</v>
+      </c>
+      <c r="C46" t="s">
+        <v>601</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1468</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E265"/>
   <sheetViews>
@@ -24262,14 +24890,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A484" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C497" sqref="C497"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48" style="87" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" style="87" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" style="87" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" style="87" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" style="87" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" style="87" customWidth="1"/>
@@ -30352,6 +30978,169 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2627</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2628</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2629</v>
+      </c>
+      <c r="B4" s="87" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B5" s="87" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>2631</v>
+      </c>
+      <c r="B6" s="87" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>2632</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>2633</v>
+      </c>
+      <c r="B8" s="87" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>2634</v>
+      </c>
+      <c r="B9" s="87" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>2635</v>
+      </c>
+      <c r="B10" s="87" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>2636</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>2638</v>
+      </c>
+      <c r="B13" s="87" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>2639</v>
+      </c>
+      <c r="B14" s="87" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>2640</v>
+      </c>
+      <c r="B15" s="87" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>2641</v>
+      </c>
+      <c r="B16" s="87" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>2642</v>
+      </c>
+      <c r="B17" s="87" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>2643</v>
+      </c>
+      <c r="B18" s="87" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView topLeftCell="A136" workbookViewId="0">
@@ -32551,7 +33340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y204"/>
   <sheetViews>
@@ -41989,7 +42778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T287"/>
   <sheetViews>
@@ -51560,7 +52349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K294"/>
   <sheetViews>
@@ -57730,7 +58519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L235"/>
   <sheetViews>
@@ -65455,7 +66244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C182"/>
   <sheetViews>
@@ -67478,577 +68267,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>503</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1549</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1550</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1551</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1552</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1554</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>342</v>
-      </c>
-      <c r="B3" t="s">
-        <v>342</v>
-      </c>
-      <c r="C3" t="s">
-        <v>602</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>339</v>
-      </c>
-      <c r="B4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1555</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>341</v>
-      </c>
-      <c r="B5" t="s">
-        <v>341</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1556</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>456</v>
-      </c>
-      <c r="B6" t="s">
-        <v>456</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1557</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>457</v>
-      </c>
-      <c r="B7" t="s">
-        <v>457</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1558</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>455</v>
-      </c>
-      <c r="B8" t="s">
-        <v>455</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1559</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>331</v>
-      </c>
-      <c r="B9" t="s">
-        <v>331</v>
-      </c>
-      <c r="C9" t="s">
-        <v>676</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>329</v>
-      </c>
-      <c r="B10" t="s">
-        <v>329</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>330</v>
-      </c>
-      <c r="B11" t="s">
-        <v>330</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>335</v>
-      </c>
-      <c r="B12" t="s">
-        <v>335</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>332</v>
-      </c>
-      <c r="B13" t="s">
-        <v>332</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>333</v>
-      </c>
-      <c r="B14" t="s">
-        <v>333</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>334</v>
-      </c>
-      <c r="B15" t="s">
-        <v>334</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>336</v>
-      </c>
-      <c r="B16" t="s">
-        <v>336</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>337</v>
-      </c>
-      <c r="B17" t="s">
-        <v>337</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>465</v>
-      </c>
-      <c r="B18" t="s">
-        <v>465</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>428</v>
-      </c>
-      <c r="B19" t="s">
-        <v>428</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>521</v>
-      </c>
-      <c r="B20" t="s">
-        <v>521</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>223</v>
-      </c>
-      <c r="B21" t="s">
-        <v>223</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>226</v>
-      </c>
-      <c r="B22" t="s">
-        <v>226</v>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>840</v>
-      </c>
-      <c r="B23" t="s">
-        <v>840</v>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>518</v>
-      </c>
-      <c r="B24" t="s">
-        <v>518</v>
-      </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>788</v>
-      </c>
-      <c r="B25" t="s">
-        <v>788</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>430</v>
-      </c>
-      <c r="B26" t="s">
-        <v>430</v>
-      </c>
-      <c r="F26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>322</v>
-      </c>
-      <c r="B27" t="s">
-        <v>322</v>
-      </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>519</v>
-      </c>
-      <c r="B28" t="s">
-        <v>519</v>
-      </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>231</v>
-      </c>
-      <c r="B29" t="s">
-        <v>231</v>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>839</v>
-      </c>
-      <c r="B30" t="s">
-        <v>839</v>
-      </c>
-      <c r="F30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>520</v>
-      </c>
-      <c r="B31" t="s">
-        <v>520</v>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>1454</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1454</v>
-      </c>
-      <c r="F32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>1480</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1480</v>
-      </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>1456</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1456</v>
-      </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>431</v>
-      </c>
-      <c r="B35" t="s">
-        <v>431</v>
-      </c>
-      <c r="F35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>786</v>
-      </c>
-      <c r="B36" t="s">
-        <v>786</v>
-      </c>
-      <c r="F36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>314</v>
-      </c>
-      <c r="B37" t="s">
-        <v>314</v>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>315</v>
-      </c>
-      <c r="B38" t="s">
-        <v>315</v>
-      </c>
-      <c r="F38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>313</v>
-      </c>
-      <c r="B39" t="s">
-        <v>313</v>
-      </c>
-      <c r="F39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>787</v>
-      </c>
-      <c r="B40" t="s">
-        <v>787</v>
-      </c>
-      <c r="F40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>523</v>
-      </c>
-      <c r="B41" t="s">
-        <v>523</v>
-      </c>
-      <c r="F41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>836</v>
-      </c>
-      <c r="B42" t="s">
-        <v>836</v>
-      </c>
-      <c r="F42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>524</v>
-      </c>
-      <c r="B43" t="s">
-        <v>524</v>
-      </c>
-      <c r="F43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>522</v>
-      </c>
-      <c r="B44" t="s">
-        <v>522</v>
-      </c>
-      <c r="F44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>807</v>
-      </c>
-      <c r="B45" t="s">
-        <v>807</v>
-      </c>
-      <c r="F45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B46" t="s">
-        <v>343</v>
-      </c>
-      <c r="C46" t="s">
-        <v>601</v>
-      </c>
-      <c r="F46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>1468</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1468</v>
-      </c>
-      <c r="F47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>